<commit_message>
Latest data Feb 2022
</commit_message>
<xml_diff>
--- a/app/data/Poker - Person Info.xlsx
+++ b/app/data/Poker - Person Info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://travack-my.sharepoint.com/personal/matthew_travack_com/Documents/Documents/Shared/Poker/Alex/01 - Jan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://travack-my.sharepoint.com/personal/matthew_travack_com/Documents/Documents/Shared/Poker/Alex/02 - Feb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEFE3A7-50FB-4EDD-B411-D1FE1F740FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52000896-89CB-4917-93C8-42A275CCD685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7727D65A-FE56-4C7B-B21F-7FFE0D737C42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>pers_firstname</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Mark</t>
   </si>
   <si>
-    <t>3,</t>
-  </si>
-  <si>
     <t>Matt</t>
   </si>
   <si>
@@ -114,15 +111,9 @@
     <t>04. Full House (3,2)</t>
   </si>
   <si>
-    <t>9,Jack,(J)</t>
-  </si>
-  <si>
     <t>Alex</t>
   </si>
   <si>
-    <t>9,</t>
-  </si>
-  <si>
     <t>Andy</t>
   </si>
   <si>
@@ -183,7 +174,10 @@
     <t>PointsBonusTotal</t>
   </si>
   <si>
-    <t>10,</t>
+    <t>8,</t>
+  </si>
+  <si>
+    <t>Ace,9,10,Jack,(9)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +532,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,19 +570,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -649,532 +643,532 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B3">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>566</v>
+        <v>109</v>
       </c>
       <c r="J3">
-        <v>3.47</v>
+        <v>4.04</v>
       </c>
       <c r="K3">
-        <v>13.08</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3">
-        <v>16.010000000000002</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I4">
-        <v>335</v>
+        <v>573</v>
       </c>
       <c r="J4">
         <v>3.49</v>
       </c>
       <c r="K4">
-        <v>16.03</v>
+        <v>13.08</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N4">
-        <v>15.09</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>422</v>
+        <v>335</v>
       </c>
       <c r="J5">
-        <v>3.64</v>
+        <v>3.49</v>
       </c>
       <c r="K5">
-        <v>14.12</v>
+        <v>16.03</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N5">
-        <v>10.11</v>
+        <v>15.09</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="E6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>586</v>
+        <v>428</v>
       </c>
       <c r="J6">
-        <v>3.71</v>
+        <v>3.66</v>
       </c>
       <c r="K6">
-        <v>13.12</v>
+        <v>14.12</v>
       </c>
       <c r="L6" t="s">
         <v>11</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N6">
-        <v>16.02</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I7">
-        <v>259</v>
+        <v>589</v>
       </c>
       <c r="J7">
-        <v>3.41</v>
+        <v>3.7</v>
       </c>
       <c r="K7">
-        <v>13.07</v>
+        <v>13.12</v>
       </c>
       <c r="L7" t="s">
         <v>11</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="N7">
-        <v>15.08</v>
+        <v>16.02</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>9</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I8">
-        <v>46</v>
+        <v>269</v>
       </c>
       <c r="J8">
-        <v>3.83</v>
+        <v>3.49</v>
       </c>
       <c r="K8">
-        <v>16.010000000000002</v>
+        <v>17.02</v>
       </c>
       <c r="L8" t="s">
         <v>11</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="N8">
-        <v>17.010000000000002</v>
+        <v>15.08</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>114</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I9">
-        <v>489</v>
+        <v>46</v>
       </c>
       <c r="J9">
-        <v>4.29</v>
+        <v>3.83</v>
       </c>
       <c r="K9">
-        <v>12.05</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="L9" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="M9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N9">
-        <v>16.11</v>
+        <v>16.010000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
         <v>12</v>
       </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I10">
-        <v>245</v>
+        <v>489</v>
       </c>
       <c r="J10">
-        <v>3.45</v>
+        <v>4.29</v>
       </c>
       <c r="K10">
-        <v>8.07</v>
+        <v>12.05</v>
       </c>
       <c r="L10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="N10">
-        <v>15.09</v>
+        <v>15.03</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>168</v>
+        <v>72</v>
       </c>
       <c r="E11">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>714</v>
+        <v>246</v>
       </c>
       <c r="J11">
-        <v>4.25</v>
+        <v>3.42</v>
       </c>
       <c r="K11">
-        <v>11.04</v>
+        <v>8.07</v>
       </c>
       <c r="L11" t="s">
         <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="N11">
-        <v>17.010000000000002</v>
+        <v>11.02</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12">
-        <v>373</v>
+        <v>714</v>
       </c>
       <c r="J12">
-        <v>3.93</v>
+        <v>4.22</v>
       </c>
       <c r="K12">
-        <v>9.08</v>
+        <v>11.04</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="N12">
-        <v>12.12</v>
+        <v>16.05</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>139</v>
+        <v>380</v>
       </c>
       <c r="J13">
-        <v>3.97</v>
+        <v>3.96</v>
       </c>
       <c r="K13">
-        <v>7.01</v>
+        <v>9.08</v>
       </c>
       <c r="L13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="M13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N13">
-        <v>10.119999999999999</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>351</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
         <v>35</v>
       </c>
-      <c r="B14">
-        <v>353</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="E14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="J14">
-        <v>3</v>
+        <v>3.97</v>
       </c>
       <c r="K14">
-        <v>5.05</v>
+        <v>7.01</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14">
+        <v>10.119999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1183,39 +1177,39 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K15">
-        <v>3.11</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>368</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D16">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <v>12</v>
@@ -1227,232 +1221,232 @@
         <v>12</v>
       </c>
       <c r="I16">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="J16">
-        <v>3.81</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="K16">
-        <v>4.0199999999999996</v>
+        <v>5.0599999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>4.0599999999999996</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I18">
-        <v>35</v>
+        <v>183</v>
       </c>
       <c r="J18">
-        <v>3.5</v>
+        <v>3.81</v>
       </c>
       <c r="K18">
-        <v>4.07</v>
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D19">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I19">
-        <v>333</v>
+        <v>5</v>
       </c>
       <c r="J19">
-        <v>3.4</v>
+        <v>2.5</v>
       </c>
       <c r="K19">
-        <v>13.04</v>
-      </c>
-      <c r="L19" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" t="s">
-        <v>12</v>
-      </c>
-      <c r="N19">
-        <v>12.05</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I20">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="J20">
-        <v>4.04</v>
+        <v>3.5</v>
       </c>
       <c r="K20">
-        <v>4.09</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I21">
-        <v>17</v>
+        <v>333</v>
       </c>
       <c r="J21">
-        <v>5.67</v>
+        <v>3.4</v>
       </c>
       <c r="K21">
-        <v>7.05</v>
+        <v>13.04</v>
+      </c>
+      <c r="L21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21">
+        <v>12.06</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>113</v>
+        <v>356</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I22">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="J22">
-        <v>5.1100000000000003</v>
+        <v>5.67</v>
       </c>
       <c r="K22">
-        <v>5.0599999999999996</v>
+        <v>7.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>